<commit_message>
Integrates StorageBOSSE in HybridBOSSE framework
</commit_message>
<xml_diff>
--- a/StorageBOSSE/test_outputs.xlsx
+++ b/StorageBOSSE/test_outputs.xlsx
@@ -344,7 +344,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1374,6 +1374,486 @@
         <v>5374259.350625235</v>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>10MW_1MWh</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>10</v>
+      </c>
+      <c r="C26" t="n">
+        <v>1</v>
+      </c>
+      <c r="D26" t="n">
+        <v>2624762.332529137</v>
+      </c>
+      <c r="E26" t="n">
+        <v>16853.27001957825</v>
+      </c>
+      <c r="F26" t="n">
+        <v>500000</v>
+      </c>
+      <c r="G26" t="n">
+        <v>1241883.500561028</v>
+      </c>
+      <c r="H26" t="n">
+        <v>333631.0619485307</v>
+      </c>
+      <c r="I26" t="n">
+        <v>25309.5</v>
+      </c>
+      <c r="J26" t="n">
+        <v>7000</v>
+      </c>
+      <c r="K26" t="n">
+        <v>2124677.332529137</v>
+      </c>
+      <c r="L26" t="n">
+        <v>500085</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>10MW_5MWh</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>10</v>
+      </c>
+      <c r="C27" t="n">
+        <v>5</v>
+      </c>
+      <c r="D27" t="n">
+        <v>3453045.992381047</v>
+      </c>
+      <c r="E27" t="n">
+        <v>16853.27001957825</v>
+      </c>
+      <c r="F27" t="n">
+        <v>500000</v>
+      </c>
+      <c r="G27" t="n">
+        <v>1241883.500561028</v>
+      </c>
+      <c r="H27" t="n">
+        <v>333631.0619485307</v>
+      </c>
+      <c r="I27" t="n">
+        <v>25309.5</v>
+      </c>
+      <c r="J27" t="n">
+        <v>7000</v>
+      </c>
+      <c r="K27" t="n">
+        <v>2124677.332529137</v>
+      </c>
+      <c r="L27" t="n">
+        <v>1328368.65985191</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>10MW_10MWh</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>10</v>
+      </c>
+      <c r="C28" t="n">
+        <v>10</v>
+      </c>
+      <c r="D28" t="n">
+        <v>4147900.680524293</v>
+      </c>
+      <c r="E28" t="n">
+        <v>16853.27001957825</v>
+      </c>
+      <c r="F28" t="n">
+        <v>500000</v>
+      </c>
+      <c r="G28" t="n">
+        <v>1241883.500561028</v>
+      </c>
+      <c r="H28" t="n">
+        <v>333631.0619485307</v>
+      </c>
+      <c r="I28" t="n">
+        <v>25309.5</v>
+      </c>
+      <c r="J28" t="n">
+        <v>7000</v>
+      </c>
+      <c r="K28" t="n">
+        <v>2124677.332529137</v>
+      </c>
+      <c r="L28" t="n">
+        <v>2023223.347995156</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>10MW_50MWh</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>10</v>
+      </c>
+      <c r="C29" t="n">
+        <v>50</v>
+      </c>
+      <c r="D29" t="n">
+        <v>8844862.020685595</v>
+      </c>
+      <c r="E29" t="n">
+        <v>35063.71975667703</v>
+      </c>
+      <c r="F29" t="n">
+        <v>500000</v>
+      </c>
+      <c r="G29" t="n">
+        <v>1241883.500561028</v>
+      </c>
+      <c r="H29" t="n">
+        <v>1584619.949742654</v>
+      </c>
+      <c r="I29" t="n">
+        <v>94035.5</v>
+      </c>
+      <c r="J29" t="n">
+        <v>15000</v>
+      </c>
+      <c r="K29" t="n">
+        <v>3470602.670060359</v>
+      </c>
+      <c r="L29" t="n">
+        <v>5374259.350625235</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>10MW_100MWh</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>10</v>
+      </c>
+      <c r="C30" t="n">
+        <v>100</v>
+      </c>
+      <c r="D30" t="n">
+        <v>13373289.64315664</v>
+      </c>
+      <c r="E30" t="n">
+        <v>58261.86192805049</v>
+      </c>
+      <c r="F30" t="n">
+        <v>500000</v>
+      </c>
+      <c r="G30" t="n">
+        <v>1241883.500561028</v>
+      </c>
+      <c r="H30" t="n">
+        <v>3182727.379485307</v>
+      </c>
+      <c r="I30" t="n">
+        <v>179943</v>
+      </c>
+      <c r="J30" t="n">
+        <v>25000</v>
+      </c>
+      <c r="K30" t="n">
+        <v>5187815.741974386</v>
+      </c>
+      <c r="L30" t="n">
+        <v>8185473.901182257</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>10MW_500MWh</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>10</v>
+      </c>
+      <c r="C31" t="n">
+        <v>500</v>
+      </c>
+      <c r="D31" t="n">
+        <v>40505105.46721184</v>
+      </c>
+      <c r="E31" t="n">
+        <v>242759.2992990382</v>
+      </c>
+      <c r="F31" t="n">
+        <v>500000</v>
+      </c>
+      <c r="G31" t="n">
+        <v>1241883.500561028</v>
+      </c>
+      <c r="H31" t="n">
+        <v>15805301.97742654</v>
+      </c>
+      <c r="I31" t="n">
+        <v>867203</v>
+      </c>
+      <c r="J31" t="n">
+        <v>105000</v>
+      </c>
+      <c r="K31" t="n">
+        <v>18762147.7772866</v>
+      </c>
+      <c r="L31" t="n">
+        <v>21742957.68992523</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>1MW_50MWh</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>1</v>
+      </c>
+      <c r="C32" t="n">
+        <v>50</v>
+      </c>
+      <c r="D32" t="n">
+        <v>7835295.448616013</v>
+      </c>
+      <c r="E32" t="n">
+        <v>35063.71975667703</v>
+      </c>
+      <c r="F32" t="n">
+        <v>500000</v>
+      </c>
+      <c r="G32" t="n">
+        <v>232316.9284914477</v>
+      </c>
+      <c r="H32" t="n">
+        <v>1584619.949742654</v>
+      </c>
+      <c r="I32" t="n">
+        <v>94035.5</v>
+      </c>
+      <c r="J32" t="n">
+        <v>15000</v>
+      </c>
+      <c r="K32" t="n">
+        <v>2461036.097990778</v>
+      </c>
+      <c r="L32" t="n">
+        <v>5374259.350625235</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>2MW_50MWh</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>2</v>
+      </c>
+      <c r="C33" t="n">
+        <v>50</v>
+      </c>
+      <c r="D33" t="n">
+        <v>7987774.64874051</v>
+      </c>
+      <c r="E33" t="n">
+        <v>35063.71975667703</v>
+      </c>
+      <c r="F33" t="n">
+        <v>500000</v>
+      </c>
+      <c r="G33" t="n">
+        <v>384796.1286159452</v>
+      </c>
+      <c r="H33" t="n">
+        <v>1584619.949742654</v>
+      </c>
+      <c r="I33" t="n">
+        <v>94035.5</v>
+      </c>
+      <c r="J33" t="n">
+        <v>15000</v>
+      </c>
+      <c r="K33" t="n">
+        <v>2613515.298115276</v>
+      </c>
+      <c r="L33" t="n">
+        <v>5374259.350625235</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>5MW_50MWh</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>5</v>
+      </c>
+      <c r="C34" t="n">
+        <v>50</v>
+      </c>
+      <c r="D34" t="n">
+        <v>8352753.632031941</v>
+      </c>
+      <c r="E34" t="n">
+        <v>35063.71975667703</v>
+      </c>
+      <c r="F34" t="n">
+        <v>500000</v>
+      </c>
+      <c r="G34" t="n">
+        <v>749775.1119073755</v>
+      </c>
+      <c r="H34" t="n">
+        <v>1584619.949742654</v>
+      </c>
+      <c r="I34" t="n">
+        <v>94035.5</v>
+      </c>
+      <c r="J34" t="n">
+        <v>15000</v>
+      </c>
+      <c r="K34" t="n">
+        <v>2978494.281406706</v>
+      </c>
+      <c r="L34" t="n">
+        <v>5374259.350625235</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>10MW_50MWh</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>10</v>
+      </c>
+      <c r="C35" t="n">
+        <v>50</v>
+      </c>
+      <c r="D35" t="n">
+        <v>8844862.020685595</v>
+      </c>
+      <c r="E35" t="n">
+        <v>35063.71975667703</v>
+      </c>
+      <c r="F35" t="n">
+        <v>500000</v>
+      </c>
+      <c r="G35" t="n">
+        <v>1241883.500561028</v>
+      </c>
+      <c r="H35" t="n">
+        <v>1584619.949742654</v>
+      </c>
+      <c r="I35" t="n">
+        <v>94035.5</v>
+      </c>
+      <c r="J35" t="n">
+        <v>15000</v>
+      </c>
+      <c r="K35" t="n">
+        <v>3470602.670060359</v>
+      </c>
+      <c r="L35" t="n">
+        <v>5374259.350625235</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>50MW_50MWh</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>50</v>
+      </c>
+      <c r="C36" t="n">
+        <v>50</v>
+      </c>
+      <c r="D36" t="n">
+        <v>10611329.06316967</v>
+      </c>
+      <c r="E36" t="n">
+        <v>35063.71975667703</v>
+      </c>
+      <c r="F36" t="n">
+        <v>2458610.043045104</v>
+      </c>
+      <c r="G36" t="n">
+        <v>1049740.5</v>
+      </c>
+      <c r="H36" t="n">
+        <v>1584619.949742654</v>
+      </c>
+      <c r="I36" t="n">
+        <v>94035.5</v>
+      </c>
+      <c r="J36" t="n">
+        <v>15000</v>
+      </c>
+      <c r="K36" t="n">
+        <v>5237069.712544435</v>
+      </c>
+      <c r="L36" t="n">
+        <v>5374259.350625235</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>100MW_50MWh</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>100</v>
+      </c>
+      <c r="C37" t="n">
+        <v>50</v>
+      </c>
+      <c r="D37" t="n">
+        <v>12826401.74351959</v>
+      </c>
+      <c r="E37" t="n">
+        <v>58261.86192805049</v>
+      </c>
+      <c r="F37" t="n">
+        <v>2956469.651481002</v>
+      </c>
+      <c r="G37" t="n">
+        <v>1049740.5</v>
+      </c>
+      <c r="H37" t="n">
+        <v>3182727.379485307</v>
+      </c>
+      <c r="I37" t="n">
+        <v>179943</v>
+      </c>
+      <c r="J37" t="n">
+        <v>25000</v>
+      </c>
+      <c r="K37" t="n">
+        <v>7452142.392894359</v>
+      </c>
+      <c r="L37" t="n">
+        <v>5374259.350625235</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>